<commit_message>
Retoques finales del proyecto
</commit_message>
<xml_diff>
--- a/API/asistencia.xlsx
+++ b/API/asistencia.xlsx
@@ -12,9 +12,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
-  <si>
-    <t>Clase de Formacion</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="32">
+  <si>
+    <t>Evento Bienestar</t>
   </si>
   <si>
     <t>Programa de formación: Analisis y desarrollo de software</t>
@@ -29,13 +29,13 @@
     <t>Sede: Centro de mantenimiento integral</t>
   </si>
   <si>
-    <t>Instructor: Juan Alfonso Torrez Perez</t>
-  </si>
-  <si>
-    <t>Clase Formacion: Desarrollo web</t>
-  </si>
-  <si>
-    <t>Fecha: 2024-10-04 00:54:34</t>
+    <t>Instructor: enzy zulay angarita bermudez</t>
+  </si>
+  <si>
+    <t>Clase Formacion: Algoritmia</t>
+  </si>
+  <si>
+    <t>Fecha: 2024-10-10 07:46:15</t>
   </si>
   <si>
     <t>#</t>
@@ -96,6 +96,18 @@
   </si>
   <si>
     <t>Santander - Bucaramanga - El Llano</t>
+  </si>
+  <si>
+    <t>0980987651</t>
+  </si>
+  <si>
+    <t>Miguel Alexander Toloza</t>
+  </si>
+  <si>
+    <t>3128765423</t>
+  </si>
+  <si>
+    <t>miguel@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -172,7 +184,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="true"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="true" applyAlignment="true">
@@ -187,13 +199,16 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
   </cellXfs>
 </styleSheet>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:H12"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -324,8 +339,34 @@
       <c r="G12" t="s" s="0">
         <v>27</v>
       </c>
-      <c r="H12" t="n" s="9">
-        <v>5.0</v>
+      <c r="H12" t="n" s="8">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n" s="0">
+        <v>3.0</v>
+      </c>
+      <c r="B13" t="s" s="0">
+        <v>28</v>
+      </c>
+      <c r="C13" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="D13" t="s" s="0">
+        <v>30</v>
+      </c>
+      <c r="E13" t="s" s="0">
+        <v>31</v>
+      </c>
+      <c r="F13" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="G13" t="s" s="0">
+        <v>21</v>
+      </c>
+      <c r="H13" t="n" s="11">
+        <v>1.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Se hicieron cambios en la api con enfoque a web
</commit_message>
<xml_diff>
--- a/API/asistencia.xlsx
+++ b/API/asistencia.xlsx
@@ -12,9 +12,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="32">
-  <si>
-    <t>Evento Bienestar</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="35">
+  <si>
+    <t>Clase de formacion</t>
   </si>
   <si>
     <t>Programa de formación: Analisis y desarrollo de software</t>
@@ -29,13 +29,13 @@
     <t>Sede: Centro de mantenimiento integral</t>
   </si>
   <si>
-    <t>Instructor: enzy zulay angarita bermudez</t>
-  </si>
-  <si>
-    <t>Clase Formacion: Algoritmia</t>
-  </si>
-  <si>
-    <t>Fecha: 2024-10-10 07:46:15</t>
+    <t>Instructor: Jhon Becerra</t>
+  </si>
+  <si>
+    <t>Clase Formacion: Desarrollo Web</t>
+  </si>
+  <si>
+    <t>Fecha: 2024-10-15 12:09:17</t>
   </si>
   <si>
     <t>#</t>
@@ -62,52 +62,61 @@
     <t>Horas de Inasistencia</t>
   </si>
   <si>
-    <t>1097096255</t>
-  </si>
-  <si>
-    <t>jeisson fernando leon avila</t>
-  </si>
-  <si>
-    <t>3168215154</t>
-  </si>
-  <si>
-    <t>jeissonfernandoleonavila@gmail.com</t>
+    <t>0987654321</t>
+  </si>
+  <si>
+    <t>Enernesto perez</t>
+  </si>
+  <si>
+    <t>111111111</t>
+  </si>
+  <si>
+    <t>ernesto@gmail.com</t>
   </si>
   <si>
     <t>Masculino</t>
   </si>
   <si>
+    <t>Santander - Bucaramanga - El Llano</t>
+  </si>
+  <si>
+    <t>1234567890</t>
+  </si>
+  <si>
+    <t>Carlos ALberto Torrez</t>
+  </si>
+  <si>
+    <t>8912381297</t>
+  </si>
+  <si>
+    <t>calberto@gmail.com</t>
+  </si>
+  <si>
     <t>Santander - Bucaramanga - La Esperanza</t>
   </si>
   <si>
-    <t>4073477</t>
-  </si>
-  <si>
-    <t>victor manuel bonilla gutierrez</t>
-  </si>
-  <si>
-    <t>3157623123</t>
-  </si>
-  <si>
-    <t>losgggg123@gmail.com</t>
-  </si>
-  <si>
-    <t>No binario</t>
-  </si>
-  <si>
-    <t>Santander - Bucaramanga - El Llano</t>
-  </si>
-  <si>
-    <t>0980987651</t>
-  </si>
-  <si>
-    <t>Miguel Alexander Toloza</t>
-  </si>
-  <si>
-    <t>3128765423</t>
-  </si>
-  <si>
-    <t>miguel@gmail.com</t>
+    <t>99999999</t>
+  </si>
+  <si>
+    <t>Pedro albaro Quinteroo</t>
+  </si>
+  <si>
+    <t>112222221</t>
+  </si>
+  <si>
+    <t>pedro@gmail.com</t>
+  </si>
+  <si>
+    <t>00000000</t>
+  </si>
+  <si>
+    <t>ejero alfredo torrez alcanso</t>
+  </si>
+  <si>
+    <t>098098098</t>
+  </si>
+  <si>
+    <t>algo@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -184,7 +193,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="true"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="true" applyAlignment="true">
@@ -202,13 +211,16 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
   </cellXfs>
 </styleSheet>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:H13"/>
+  <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -216,10 +228,10 @@
   <cols>
     <col min="1" max="1" width="2.34375" customWidth="true" bestFit="true"/>
     <col min="2" max="2" width="12.81640625" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="28.41015625" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="25.6953125" customWidth="true" bestFit="true"/>
     <col min="4" max="4" width="12.1875" customWidth="true" bestFit="true"/>
-    <col min="5" max="5" width="34.66796875" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="10.41796875" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="19.66796875" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="10.24609375" customWidth="true" bestFit="true"/>
     <col min="7" max="7" width="37.33203125" customWidth="true" bestFit="true"/>
     <col min="8" max="8" width="22.25390625" customWidth="true" bestFit="true"/>
   </cols>
@@ -334,13 +346,13 @@
         <v>25</v>
       </c>
       <c r="F12" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="G12" t="s" s="0">
         <v>26</v>
       </c>
-      <c r="G12" t="s" s="0">
-        <v>27</v>
-      </c>
-      <c r="H12" t="n" s="8">
-        <v>1.0</v>
+      <c r="H12" t="n" s="7">
+        <v>0.0</v>
       </c>
     </row>
     <row r="13">
@@ -348,16 +360,16 @@
         <v>3.0</v>
       </c>
       <c r="B13" t="s" s="0">
+        <v>27</v>
+      </c>
+      <c r="C13" t="s" s="0">
         <v>28</v>
       </c>
-      <c r="C13" t="s" s="0">
+      <c r="D13" t="s" s="0">
         <v>29</v>
       </c>
-      <c r="D13" t="s" s="0">
+      <c r="E13" t="s" s="0">
         <v>30</v>
-      </c>
-      <c r="E13" t="s" s="0">
-        <v>31</v>
       </c>
       <c r="F13" t="s" s="0">
         <v>20</v>
@@ -365,8 +377,34 @@
       <c r="G13" t="s" s="0">
         <v>21</v>
       </c>
-      <c r="H13" t="n" s="11">
-        <v>1.0</v>
+      <c r="H13" t="n" s="12">
+        <v>5.0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n" s="0">
+        <v>4.0</v>
+      </c>
+      <c r="B14" t="s" s="0">
+        <v>31</v>
+      </c>
+      <c r="C14" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="D14" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="E14" t="s" s="0">
+        <v>34</v>
+      </c>
+      <c r="F14" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="G14" t="s" s="0">
+        <v>21</v>
+      </c>
+      <c r="H14" t="n" s="15">
+        <v>5.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>